<commit_message>
[master] Add Tutorial9, Add csv file for Tutorial8
</commit_message>
<xml_diff>
--- a/tutorials/tutorial_8/resources/SampleData.xlsx
+++ b/tutorials/tutorial_8/resources/SampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Apache24\htdocs\php_training\tutorials\tutorial_8\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49644622-5E72-44CD-A738-C15206B60547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEED4F5-4FED-4A4F-8AE9-0EE2B3AF2AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -221,7 +221,7 @@
     <t>Get emails with Excel tips, links, and news</t>
   </si>
   <si>
-    <t>z</t>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -615,7 +615,7 @@
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Item"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Units"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="z"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="total"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1086,7 +1086,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>